<commit_message>
Final Universal code edit
</commit_message>
<xml_diff>
--- a/Facility_by_state.xlsx
+++ b/Facility_by_state.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keros\.venv\Capstone-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kelly's Education Folder\Data Analytics Capstone\Research Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{273B1083-4E0E-40C0-8CB7-E2267FFBC441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7F68E9B-93F3-44B5-B994-52D21619A5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320"/>
   </bookViews>
@@ -506,8 +506,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -863,9 +866,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A53"/>
+  <dimension ref="A1:A55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -879,263 +884,261 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>15003</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>225</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>20</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>142</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>218</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1170</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>203</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>17</v>
+        <v>697</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>697</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>357</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>43</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>80</v>
+        <v>694</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>694</v>
+        <v>521</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>521</v>
+        <v>412</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>412</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>313</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>269</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>87</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>225</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>353</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>430</v>
+        <v>353</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>353</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>202</v>
+        <v>510</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>510</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>62</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>185</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>73</v>
+        <v>348</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>348</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>68</v>
+        <v>606</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>606</v>
+        <v>420</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>420</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>77</v>
+        <v>946</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>946</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>292</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>129</v>
+        <v>672</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>672</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>75</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>188</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>98</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>312</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>1195</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>98</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>35</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>289</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>198</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>123</v>
+        <v>332</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
         <v>36</v>
       </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>